<commit_message>
Now with a more complete watch and station bill in the output.
</commit_message>
<xml_diff>
--- a/poc/jc_skills_grid.xlsx
+++ b/poc/jc_skills_grid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38300" windowHeight="25300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38300" windowHeight="25300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Skills Grid" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="506">
   <si>
     <t>Respond to an MOB</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1714,9 +1714,6 @@
   </si>
   <si>
     <t>MS-M4</t>
-  </si>
-  <si>
-    <t>MS-M9</t>
   </si>
   <si>
     <t>MS-F1</t>
@@ -4258,11 +4255,11 @@
   </sheetPr>
   <dimension ref="A1:JJ132"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="DT4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="EN9" sqref="EN9"/>
+      <selection pane="bottomRight" activeCell="FC7" sqref="FC7:FG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -7218,35 +7215,25 @@
       <c r="EZ7" s="14"/>
       <c r="FA7" s="9"/>
       <c r="FB7" s="10"/>
-      <c r="FC7" s="9" t="s">
+      <c r="FC7" s="9"/>
+      <c r="FD7" s="9"/>
+      <c r="FE7" s="9"/>
+      <c r="FF7" s="9"/>
+      <c r="FG7" s="9"/>
+      <c r="FH7" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="FD7" s="9" t="s">
+      <c r="FI7" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="FE7" s="9" t="s">
+      <c r="FJ7" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="FF7" s="9" t="s">
+      <c r="FK7" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="FG7" s="9" t="s">
+      <c r="FL7" s="9" t="s">
         <v>491</v>
-      </c>
-      <c r="FH7" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="FI7" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="FJ7" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="FK7" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="FL7" s="9" t="s">
-        <v>492</v>
       </c>
       <c r="FM7" s="9"/>
       <c r="FN7" s="9"/>
@@ -7259,7 +7246,7 @@
       <c r="FU7" s="9"/>
       <c r="FV7" s="9"/>
       <c r="FW7" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="FX7" s="9"/>
       <c r="FY7" s="9"/>
@@ -7273,17 +7260,17 @@
       <c r="GG7" s="9"/>
       <c r="GH7" s="9"/>
       <c r="GI7" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="GJ7" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="GK7" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="GL7" s="9"/>
       <c r="GM7" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="GN7" s="9"/>
       <c r="GO7" s="9"/>
@@ -7302,16 +7289,16 @@
       <c r="HB7" s="9"/>
       <c r="HC7" s="9"/>
       <c r="HD7" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="HH7" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="HH7" s="2" t="s">
+      <c r="HK7" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="HK7" s="2" t="s">
-        <v>500</v>
-      </c>
       <c r="HN7" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="8" spans="1:270" s="31" customFormat="1" ht="14">
@@ -30899,11 +30886,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q1:Q1048576"/>
+      <selection pane="bottomRight" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -34869,7 +34856,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1:J1048576"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -34897,7 +34884,7 @@
       </c>
       <c r="D2" s="16">
         <f>COUNTIF(D5:D67,"Y")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -34946,7 +34933,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B5" s="84" t="s">
         <v>381</v>
@@ -34973,7 +34960,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B6" s="68" t="s">
         <v>382</v>
@@ -35087,7 +35074,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B11" s="67" t="s">
         <v>380</v>
@@ -35118,7 +35105,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B12" s="67" t="s">
         <v>429</v>
@@ -35222,7 +35209,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B16" s="72" t="s">
         <v>431</v>
@@ -35287,7 +35274,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B19" s="72" t="s">
         <v>432</v>
@@ -35310,7 +35297,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B20" s="72" t="s">
         <v>432</v>
@@ -35331,7 +35318,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B21" s="72" t="s">
         <v>432</v>
@@ -35436,7 +35423,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B26" s="67" t="s">
         <v>433</v>
@@ -35461,7 +35448,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B27" s="67" t="s">
         <v>433</v>
@@ -35486,7 +35473,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B28" s="67" t="s">
         <v>433</v>
@@ -35511,7 +35498,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B29" s="67" t="s">
         <v>433</v>
@@ -36002,7 +35989,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>457</v>
+        <v>498</v>
       </c>
       <c r="B52" s="67" t="s">
         <v>383</v>
@@ -36010,7 +35997,7 @@
       <c r="C52" s="98"/>
       <c r="D52" s="52" t="str">
         <f t="array" ref="D52">IF(OR(ISNUMBER(SEARCH(","&amp;$A52&amp;",",","&amp;WnSAssignmentMoveShip&amp;","))),"Y","-")</f>
-        <v>-</v>
+        <v>Y</v>
       </c>
       <c r="E52" s="53">
         <v>4</v>
@@ -44962,9 +44949,9 @@
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
         <v>0</v>
       </c>
-      <c r="G158" t="str">
-        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
-        <v>MS-M9</v>
+      <c r="G158">
+        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
+        <v>0</v>
       </c>
       <c r="H158" t="str">
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
@@ -44996,9 +44983,9 @@
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
         <v>0</v>
       </c>
-      <c r="G159" t="str">
-        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
-        <v>MS-M9</v>
+      <c r="G159">
+        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
+        <v>0</v>
       </c>
       <c r="H159" t="str">
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
@@ -45030,9 +45017,9 @@
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
         <v>0</v>
       </c>
-      <c r="G160" t="str">
-        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
-        <v>MS-M9</v>
+      <c r="G160">
+        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
+        <v>0</v>
       </c>
       <c r="H160" t="str">
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
@@ -45064,9 +45051,9 @@
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
         <v>0</v>
       </c>
-      <c r="G161" t="str">
-        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
-        <v>MS-M9</v>
+      <c r="G161">
+        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
+        <v>0</v>
       </c>
       <c r="H161" t="str">
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
@@ -45098,9 +45085,9 @@
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
         <v>0</v>
       </c>
-      <c r="G162" t="str">
-        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
-        <v>MS-M9</v>
+      <c r="G162">
+        <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>
+        <v>0</v>
       </c>
       <c r="H162" t="str">
         <f ca="1">OFFSET('Skills Grid'!$C$1,COLUMN()-COLUMN($A$2),ROW()-ROW($D$2))</f>

</xml_diff>